<commit_message>
modify bins translation and UI
</commit_message>
<xml_diff>
--- a/inst/app/www/meta/lable_info.xlsx
+++ b/inst/app/www/meta/lable_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/choonghyunryu/Documents/01_Personal/00_bitr/01_packages/BitStat/inst/app/www/meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B7B0C8-D3DE-EA43-8AC5-8750E0D38455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F7F386-CABF-A24B-AB89-B68A02BCA413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15420" yWindow="6480" windowWidth="33600" windowHeight="19500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="시트 1 - lable_info" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1223" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1272" uniqueCount="462">
   <si>
     <t>no</t>
   </si>
@@ -1465,6 +1465,46 @@
   <si>
     <t>Number of bins:</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bin_distribution의 element</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>치솟값</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5%분위</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10%분위</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1/4분위</t>
+  </si>
+  <si>
+    <t>중위수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>산술평균</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3/4분위</t>
+  </si>
+  <si>
+    <t>90%분위</t>
+  </si>
+  <si>
+    <t>95%분위</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>최댓값</t>
   </si>
 </sst>
 </file>
@@ -2832,10 +2872,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J147"/>
+  <dimension ref="A1:J157"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="F129" sqref="F129"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="A132" sqref="A132:A157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1"/>
@@ -7110,76 +7150,86 @@
         <v>59</v>
       </c>
       <c r="E136" s="9" t="s">
-        <v>439</v>
-      </c>
-      <c r="F136" s="9" t="s">
-        <v>440</v>
-      </c>
-      <c r="G136" s="10" t="s">
-        <v>437</v>
-      </c>
+        <v>452</v>
+      </c>
+      <c r="F136" s="9"/>
+      <c r="G136" s="10"/>
       <c r="H136" s="9"/>
-      <c r="I136" s="10" t="s">
-        <v>355</v>
-      </c>
+      <c r="I136" s="10"/>
       <c r="J136" s="9" t="s">
-        <v>442</v>
+        <v>451</v>
       </c>
     </row>
     <row r="137" spans="1:10" ht="20" customHeight="1">
       <c r="A137" s="7">
         <v>136</v>
       </c>
-      <c r="B137" s="8"/>
-      <c r="C137" s="10"/>
-      <c r="D137" s="10"/>
-      <c r="E137" s="9"/>
+      <c r="B137" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C137" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D137" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E137" s="9" t="s">
+        <v>453</v>
+      </c>
       <c r="F137" s="9"/>
       <c r="G137" s="10"/>
       <c r="H137" s="9"/>
       <c r="I137" s="10"/>
-      <c r="J137" s="9"/>
+      <c r="J137" s="9" t="s">
+        <v>451</v>
+      </c>
     </row>
     <row r="138" spans="1:10" ht="20" customHeight="1">
       <c r="A138" s="7">
         <v>137</v>
       </c>
-      <c r="B138" s="8"/>
-      <c r="C138" s="10"/>
-      <c r="D138" s="10"/>
-      <c r="E138" s="9"/>
+      <c r="B138" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C138" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D138" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E138" s="9" t="s">
+        <v>454</v>
+      </c>
       <c r="F138" s="9"/>
       <c r="G138" s="10"/>
       <c r="H138" s="9"/>
       <c r="I138" s="10"/>
-      <c r="J138" s="9"/>
+      <c r="J138" s="9" t="s">
+        <v>451</v>
+      </c>
     </row>
     <row r="139" spans="1:10" ht="20" customHeight="1">
       <c r="A139" s="7">
         <v>138</v>
       </c>
       <c r="B139" s="8" t="s">
-        <v>389</v>
+        <v>16</v>
       </c>
       <c r="C139" s="10" t="s">
-        <v>390</v>
-      </c>
-      <c r="D139" s="10"/>
+        <v>44</v>
+      </c>
+      <c r="D139" s="10" t="s">
+        <v>59</v>
+      </c>
       <c r="E139" s="9" t="s">
-        <v>396</v>
-      </c>
-      <c r="F139" s="9" t="s">
-        <v>393</v>
-      </c>
+        <v>455</v>
+      </c>
+      <c r="F139" s="9"/>
       <c r="G139" s="10"/>
-      <c r="H139" s="9" t="s">
-        <v>391</v>
-      </c>
-      <c r="I139" s="10" t="s">
-        <v>355</v>
-      </c>
+      <c r="H139" s="9"/>
+      <c r="I139" s="10"/>
       <c r="J139" s="9" t="s">
-        <v>390</v>
+        <v>451</v>
       </c>
     </row>
     <row r="140" spans="1:10" ht="20" customHeight="1">
@@ -7187,27 +7237,23 @@
         <v>139</v>
       </c>
       <c r="B140" s="8" t="s">
-        <v>389</v>
+        <v>16</v>
       </c>
       <c r="C140" s="10" t="s">
-        <v>390</v>
-      </c>
-      <c r="D140" s="10"/>
+        <v>44</v>
+      </c>
+      <c r="D140" s="10" t="s">
+        <v>59</v>
+      </c>
       <c r="E140" s="9" t="s">
-        <v>397</v>
-      </c>
-      <c r="F140" s="9" t="s">
-        <v>394</v>
-      </c>
+        <v>456</v>
+      </c>
+      <c r="F140" s="9"/>
       <c r="G140" s="10"/>
-      <c r="H140" s="9" t="s">
-        <v>391</v>
-      </c>
-      <c r="I140" s="10" t="s">
-        <v>355</v>
-      </c>
+      <c r="H140" s="9"/>
+      <c r="I140" s="10"/>
       <c r="J140" s="9" t="s">
-        <v>390</v>
+        <v>451</v>
       </c>
     </row>
     <row r="141" spans="1:10" ht="20" customHeight="1">
@@ -7215,27 +7261,23 @@
         <v>140</v>
       </c>
       <c r="B141" s="8" t="s">
-        <v>389</v>
+        <v>16</v>
       </c>
       <c r="C141" s="10" t="s">
-        <v>390</v>
-      </c>
-      <c r="D141" s="10"/>
+        <v>44</v>
+      </c>
+      <c r="D141" s="10" t="s">
+        <v>59</v>
+      </c>
       <c r="E141" s="9" t="s">
-        <v>392</v>
-      </c>
-      <c r="F141" s="9" t="s">
-        <v>395</v>
-      </c>
+        <v>457</v>
+      </c>
+      <c r="F141" s="9"/>
       <c r="G141" s="10"/>
-      <c r="H141" s="9" t="s">
-        <v>391</v>
-      </c>
-      <c r="I141" s="10" t="s">
-        <v>355</v>
-      </c>
+      <c r="H141" s="9"/>
+      <c r="I141" s="10"/>
       <c r="J141" s="9" t="s">
-        <v>390</v>
+        <v>451</v>
       </c>
     </row>
     <row r="142" spans="1:10" ht="20" customHeight="1">
@@ -7243,27 +7285,23 @@
         <v>141</v>
       </c>
       <c r="B142" s="8" t="s">
-        <v>389</v>
+        <v>16</v>
       </c>
       <c r="C142" s="10" t="s">
-        <v>390</v>
-      </c>
-      <c r="D142" s="10"/>
+        <v>44</v>
+      </c>
+      <c r="D142" s="10" t="s">
+        <v>59</v>
+      </c>
       <c r="E142" s="9" t="s">
-        <v>399</v>
-      </c>
-      <c r="F142" s="9" t="s">
-        <v>400</v>
-      </c>
+        <v>458</v>
+      </c>
+      <c r="F142" s="9"/>
       <c r="G142" s="10"/>
-      <c r="H142" s="9" t="s">
-        <v>391</v>
-      </c>
-      <c r="I142" s="10" t="s">
-        <v>355</v>
-      </c>
+      <c r="H142" s="9"/>
+      <c r="I142" s="10"/>
       <c r="J142" s="9" t="s">
-        <v>390</v>
+        <v>451</v>
       </c>
     </row>
     <row r="143" spans="1:10" ht="20" customHeight="1">
@@ -7271,41 +7309,65 @@
         <v>142</v>
       </c>
       <c r="B143" s="8" t="s">
-        <v>389</v>
+        <v>16</v>
       </c>
       <c r="C143" s="10" t="s">
-        <v>390</v>
-      </c>
-      <c r="D143" s="10"/>
-      <c r="E143" s="9"/>
+        <v>44</v>
+      </c>
+      <c r="D143" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E143" s="9" t="s">
+        <v>459</v>
+      </c>
       <c r="F143" s="9"/>
       <c r="G143" s="10"/>
       <c r="H143" s="9"/>
       <c r="I143" s="10"/>
-      <c r="J143" s="9"/>
+      <c r="J143" s="9" t="s">
+        <v>451</v>
+      </c>
     </row>
     <row r="144" spans="1:10" ht="20" customHeight="1">
       <c r="A144" s="7">
         <v>143</v>
       </c>
-      <c r="B144" s="8"/>
-      <c r="C144" s="10"/>
-      <c r="D144" s="10"/>
-      <c r="E144" s="9"/>
+      <c r="B144" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C144" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D144" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E144" s="9" t="s">
+        <v>460</v>
+      </c>
       <c r="F144" s="9"/>
       <c r="G144" s="10"/>
       <c r="H144" s="9"/>
       <c r="I144" s="10"/>
-      <c r="J144" s="9"/>
+      <c r="J144" s="9" t="s">
+        <v>451</v>
+      </c>
     </row>
     <row r="145" spans="1:10" ht="20" customHeight="1">
       <c r="A145" s="7">
         <v>144</v>
       </c>
-      <c r="B145" s="8"/>
-      <c r="C145" s="10"/>
-      <c r="D145" s="10"/>
-      <c r="E145" s="9"/>
+      <c r="B145" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C145" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D145" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E145" s="9" t="s">
+        <v>461</v>
+      </c>
       <c r="F145" s="9"/>
       <c r="G145" s="10"/>
       <c r="H145" s="9"/>
@@ -7316,43 +7378,259 @@
       <c r="A146" s="7">
         <v>145</v>
       </c>
-      <c r="B146" s="8"/>
-      <c r="C146" s="10"/>
-      <c r="D146" s="10"/>
-      <c r="E146" s="9"/>
-      <c r="F146" s="9"/>
-      <c r="G146" s="10"/>
+      <c r="B146" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C146" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D146" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E146" s="9" t="s">
+        <v>439</v>
+      </c>
+      <c r="F146" s="9" t="s">
+        <v>440</v>
+      </c>
+      <c r="G146" s="10" t="s">
+        <v>437</v>
+      </c>
       <c r="H146" s="9"/>
-      <c r="I146" s="10"/>
-      <c r="J146" s="9"/>
+      <c r="I146" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="J146" s="9" t="s">
+        <v>442</v>
+      </c>
     </row>
     <row r="147" spans="1:10" ht="20" customHeight="1">
       <c r="A147" s="7">
         <v>146</v>
       </c>
-      <c r="B147" s="8" t="s">
+      <c r="B147" s="8"/>
+      <c r="C147" s="10"/>
+      <c r="D147" s="10"/>
+      <c r="E147" s="9"/>
+      <c r="F147" s="9"/>
+      <c r="G147" s="10"/>
+      <c r="H147" s="9"/>
+      <c r="I147" s="10"/>
+      <c r="J147" s="9"/>
+    </row>
+    <row r="148" spans="1:10" ht="20" customHeight="1">
+      <c r="A148" s="7">
+        <v>147</v>
+      </c>
+      <c r="B148" s="8"/>
+      <c r="C148" s="10"/>
+      <c r="D148" s="10"/>
+      <c r="E148" s="9"/>
+      <c r="F148" s="9"/>
+      <c r="G148" s="10"/>
+      <c r="H148" s="9"/>
+      <c r="I148" s="10"/>
+      <c r="J148" s="9"/>
+    </row>
+    <row r="149" spans="1:10" ht="20" customHeight="1">
+      <c r="A149" s="7">
+        <v>148</v>
+      </c>
+      <c r="B149" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="C149" s="10" t="s">
+        <v>390</v>
+      </c>
+      <c r="D149" s="10"/>
+      <c r="E149" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="F149" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="G149" s="10"/>
+      <c r="H149" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="I149" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="J149" s="9" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" ht="20" customHeight="1">
+      <c r="A150" s="7">
+        <v>149</v>
+      </c>
+      <c r="B150" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="C150" s="10" t="s">
+        <v>390</v>
+      </c>
+      <c r="D150" s="10"/>
+      <c r="E150" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="F150" s="9" t="s">
+        <v>394</v>
+      </c>
+      <c r="G150" s="10"/>
+      <c r="H150" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="I150" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="J150" s="9" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" ht="20" customHeight="1">
+      <c r="A151" s="7">
+        <v>150</v>
+      </c>
+      <c r="B151" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="C151" s="10" t="s">
+        <v>390</v>
+      </c>
+      <c r="D151" s="10"/>
+      <c r="E151" s="9" t="s">
+        <v>392</v>
+      </c>
+      <c r="F151" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="G151" s="10"/>
+      <c r="H151" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="I151" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="J151" s="9" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" ht="20" customHeight="1">
+      <c r="A152" s="7">
+        <v>151</v>
+      </c>
+      <c r="B152" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="C152" s="10" t="s">
+        <v>390</v>
+      </c>
+      <c r="D152" s="10"/>
+      <c r="E152" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="F152" s="9" t="s">
+        <v>400</v>
+      </c>
+      <c r="G152" s="10"/>
+      <c r="H152" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="I152" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="J152" s="9" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" ht="20" customHeight="1">
+      <c r="A153" s="7">
+        <v>152</v>
+      </c>
+      <c r="B153" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="C153" s="10" t="s">
+        <v>390</v>
+      </c>
+      <c r="D153" s="10"/>
+      <c r="E153" s="9"/>
+      <c r="F153" s="9"/>
+      <c r="G153" s="10"/>
+      <c r="H153" s="9"/>
+      <c r="I153" s="10"/>
+      <c r="J153" s="9"/>
+    </row>
+    <row r="154" spans="1:10" ht="20" customHeight="1">
+      <c r="A154" s="7">
+        <v>153</v>
+      </c>
+      <c r="B154" s="8"/>
+      <c r="C154" s="10"/>
+      <c r="D154" s="10"/>
+      <c r="E154" s="9"/>
+      <c r="F154" s="9"/>
+      <c r="G154" s="10"/>
+      <c r="H154" s="9"/>
+      <c r="I154" s="10"/>
+      <c r="J154" s="9"/>
+    </row>
+    <row r="155" spans="1:10" ht="20" customHeight="1">
+      <c r="A155" s="7">
+        <v>154</v>
+      </c>
+      <c r="B155" s="8"/>
+      <c r="C155" s="10"/>
+      <c r="D155" s="10"/>
+      <c r="E155" s="9"/>
+      <c r="F155" s="9"/>
+      <c r="G155" s="10"/>
+      <c r="H155" s="9"/>
+      <c r="I155" s="10"/>
+      <c r="J155" s="9"/>
+    </row>
+    <row r="156" spans="1:10" ht="20" customHeight="1">
+      <c r="A156" s="7">
+        <v>155</v>
+      </c>
+      <c r="B156" s="8"/>
+      <c r="C156" s="10"/>
+      <c r="D156" s="10"/>
+      <c r="E156" s="9"/>
+      <c r="F156" s="9"/>
+      <c r="G156" s="10"/>
+      <c r="H156" s="9"/>
+      <c r="I156" s="10"/>
+      <c r="J156" s="9"/>
+    </row>
+    <row r="157" spans="1:10" ht="20" customHeight="1">
+      <c r="A157" s="7">
+        <v>156</v>
+      </c>
+      <c r="B157" s="8" t="s">
         <v>316</v>
       </c>
-      <c r="C147" s="10" t="s">
+      <c r="C157" s="10" t="s">
         <v>317</v>
       </c>
-      <c r="D147" s="9"/>
-      <c r="E147" s="10" t="s">
+      <c r="D157" s="9"/>
+      <c r="E157" s="10" t="s">
         <v>318</v>
       </c>
-      <c r="F147" s="10" t="s">
+      <c r="F157" s="10" t="s">
         <v>319</v>
       </c>
-      <c r="G147" s="10" t="s">
+      <c r="G157" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H147" s="10" t="s">
+      <c r="H157" s="10" t="s">
         <v>320</v>
       </c>
-      <c r="I147" s="10" t="s">
+      <c r="I157" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="J147" s="10" t="s">
+      <c r="J157" s="10" t="s">
         <v>321</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finish Frequency Table of Categorical Variables
</commit_message>
<xml_diff>
--- a/inst/app/www/meta/lable_info.xlsx
+++ b/inst/app/www/meta/lable_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/choonghyunryu/Documents/01_Personal/00_bitr/01_packages/BitStat/inst/app/www/meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735D42EC-D86B-F047-B3B0-255EE8CF55B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6E048F-0420-FA44-B247-7CC90CE8337F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lable_info" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2611" uniqueCount="777">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2717" uniqueCount="799">
   <si>
     <t>메뉴</t>
   </si>
@@ -2290,10 +2290,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Summary_numeric.Rmd의 청크 내 정의</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>상관행렬</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2659,6 +2655,83 @@
   </si>
   <si>
     <t>calculate by category is checked, but categorical variables is not selected. Uncheck or select a variable.</t>
+  </si>
+  <si>
+    <t>수치형 변수 통계표</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>범주형 변수 돗수분포표</t>
+  </si>
+  <si>
+    <t>대상변수 선택 방법:</t>
+  </si>
+  <si>
+    <t>choice_categorical_table</t>
+  </si>
+  <si>
+    <t>list_cat_var_table</t>
+  </si>
+  <si>
+    <t>choice_categorical_table</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>choice_categorical_table의 element</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>범주형 변수 목록(하나이상 선택)</t>
+  </si>
+  <si>
+    <t>Categorical Variables(Choose one or more):</t>
+  </si>
+  <si>
+    <t>viz_cat_table</t>
+  </si>
+  <si>
+    <t>범주형 변수는 1개 이상을 선택해야 합니다.</t>
+  </si>
+  <si>
+    <t>runCategoricalSummary</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>runCategoricalSummary의 observeEvent에서 사용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>You must select at least one categorical variables.</t>
+  </si>
+  <si>
+    <t>범주형 변수 집계 테이블</t>
+  </si>
+  <si>
+    <t>Summary Table of Categorical Variables</t>
+  </si>
+  <si>
+    <t>돗수분포표</t>
+  </si>
+  <si>
+    <t>Frequency Table</t>
+  </si>
+  <si>
+    <t>범주형 변수 플롯</t>
+  </si>
+  <si>
+    <t>Plot of Categorical Variables</t>
+  </si>
+  <si>
+    <t>summary_category.Rmd의 청크 내 정의</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>summary_numeric.Rmd의 청크 내 정의</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>caption</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -4128,11 +4201,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K267"/>
+  <dimension ref="A1:K278"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A147" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F270" sqref="F270"/>
+      <pane ySplit="1" topLeftCell="A255" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A214" sqref="A214:A278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1"/>
@@ -10208,7 +10281,7 @@
         <v>560</v>
       </c>
       <c r="D176" s="26" t="s">
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E176" s="16" t="s">
         <v>558</v>
@@ -10241,7 +10314,7 @@
         <v>560</v>
       </c>
       <c r="D177" s="26" t="s">
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E177" s="16" t="s">
         <v>558</v>
@@ -10276,7 +10349,7 @@
         <v>560</v>
       </c>
       <c r="D178" s="26" t="s">
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E178" s="16" t="s">
         <v>558</v>
@@ -10311,7 +10384,7 @@
         <v>560</v>
       </c>
       <c r="D179" s="26" t="s">
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E179" s="16" t="s">
         <v>558</v>
@@ -10346,7 +10419,7 @@
         <v>560</v>
       </c>
       <c r="D180" s="26" t="s">
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E180" s="16" t="s">
         <v>558</v>
@@ -10381,7 +10454,7 @@
         <v>560</v>
       </c>
       <c r="D181" s="26" t="s">
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E181" s="16" t="s">
         <v>558</v>
@@ -10416,7 +10489,7 @@
         <v>560</v>
       </c>
       <c r="D182" s="26" t="s">
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E182" s="16" t="s">
         <v>558</v>
@@ -10451,7 +10524,7 @@
         <v>560</v>
       </c>
       <c r="D183" s="26" t="s">
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E183" s="16" t="s">
         <v>558</v>
@@ -10486,7 +10559,7 @@
         <v>560</v>
       </c>
       <c r="D184" s="26" t="s">
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E184" s="16" t="s">
         <v>558</v>
@@ -10521,7 +10594,7 @@
         <v>560</v>
       </c>
       <c r="D185" s="26" t="s">
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E185" s="16" t="s">
         <v>558</v>
@@ -10556,7 +10629,7 @@
         <v>560</v>
       </c>
       <c r="D186" s="26" t="s">
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E186" s="16" t="s">
         <v>558</v>
@@ -10591,7 +10664,7 @@
         <v>560</v>
       </c>
       <c r="D187" s="26" t="s">
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E187" s="16" t="s">
         <v>558</v>
@@ -10626,7 +10699,7 @@
         <v>560</v>
       </c>
       <c r="D188" s="26" t="s">
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E188" s="16" t="s">
         <v>558</v>
@@ -10661,7 +10734,7 @@
         <v>560</v>
       </c>
       <c r="D189" s="26" t="s">
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E189" s="16" t="s">
         <v>558</v>
@@ -10696,7 +10769,7 @@
         <v>560</v>
       </c>
       <c r="D190" s="26" t="s">
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E190" s="16" t="s">
         <v>558</v>
@@ -10731,7 +10804,7 @@
         <v>560</v>
       </c>
       <c r="D191" s="26" t="s">
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E191" s="16" t="s">
         <v>558</v>
@@ -10766,7 +10839,7 @@
         <v>560</v>
       </c>
       <c r="D192" s="26" t="s">
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E192" s="16" t="s">
         <v>558</v>
@@ -10801,7 +10874,7 @@
         <v>560</v>
       </c>
       <c r="D193" s="26" t="s">
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E193" s="16" t="s">
         <v>558</v>
@@ -10836,7 +10909,7 @@
         <v>560</v>
       </c>
       <c r="D194" s="26" t="s">
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E194" s="16" t="s">
         <v>558</v>
@@ -10871,7 +10944,7 @@
         <v>560</v>
       </c>
       <c r="D195" s="26" t="s">
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E195" s="16" t="s">
         <v>558</v>
@@ -10906,7 +10979,7 @@
         <v>560</v>
       </c>
       <c r="D196" s="26" t="s">
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E196" s="16" t="s">
         <v>558</v>
@@ -10941,7 +11014,7 @@
         <v>560</v>
       </c>
       <c r="D197" s="26" t="s">
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E197" s="16" t="s">
         <v>558</v>
@@ -10976,7 +11049,7 @@
         <v>560</v>
       </c>
       <c r="D198" s="26" t="s">
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E198" s="16" t="s">
         <v>558</v>
@@ -11011,7 +11084,7 @@
         <v>560</v>
       </c>
       <c r="D199" s="26" t="s">
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E199" s="16" t="s">
         <v>558</v>
@@ -11046,7 +11119,7 @@
         <v>560</v>
       </c>
       <c r="D200" s="26" t="s">
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E200" s="16" t="s">
         <v>558</v>
@@ -11081,7 +11154,7 @@
         <v>560</v>
       </c>
       <c r="D201" s="26" t="s">
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E201" s="16" t="s">
         <v>558</v>
@@ -11116,7 +11189,7 @@
         <v>560</v>
       </c>
       <c r="D202" s="26" t="s">
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E202" s="16" t="s">
         <v>558</v>
@@ -11151,7 +11224,7 @@
         <v>560</v>
       </c>
       <c r="D203" s="26" t="s">
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E203" s="16" t="s">
         <v>558</v>
@@ -11186,7 +11259,7 @@
         <v>560</v>
       </c>
       <c r="D204" s="26" t="s">
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E204" s="16" t="s">
         <v>558</v>
@@ -11221,7 +11294,7 @@
         <v>560</v>
       </c>
       <c r="D205" s="26" t="s">
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E205" s="16" t="s">
         <v>558</v>
@@ -11256,7 +11329,7 @@
         <v>560</v>
       </c>
       <c r="D206" s="26" t="s">
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E206" s="16" t="s">
         <v>558</v>
@@ -11291,7 +11364,7 @@
         <v>560</v>
       </c>
       <c r="D207" s="26" t="s">
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E207" s="16" t="s">
         <v>558</v>
@@ -11326,7 +11399,7 @@
         <v>560</v>
       </c>
       <c r="D208" s="26" t="s">
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E208" s="16" t="s">
         <v>558</v>
@@ -11361,7 +11434,7 @@
         <v>560</v>
       </c>
       <c r="D209" s="26" t="s">
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E209" s="16" t="s">
         <v>558</v>
@@ -11396,28 +11469,28 @@
         <v>560</v>
       </c>
       <c r="D210" s="26" t="s">
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E210" s="16" t="s">
         <v>558</v>
       </c>
       <c r="F210" s="21" t="s">
+        <v>685</v>
+      </c>
+      <c r="G210" s="21" t="s">
         <v>686</v>
-      </c>
-      <c r="G210" s="21" t="s">
-        <v>687</v>
       </c>
       <c r="H210" s="9" t="s">
         <v>70</v>
       </c>
       <c r="I210" s="8" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="J210" s="9" t="s">
         <v>394</v>
       </c>
       <c r="K210" s="8" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="211" spans="1:11" ht="20" customHeight="1">
@@ -11431,28 +11504,28 @@
         <v>560</v>
       </c>
       <c r="D211" s="26" t="s">
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E211" s="16" t="s">
         <v>558</v>
       </c>
       <c r="F211" s="21" t="s">
+        <v>689</v>
+      </c>
+      <c r="G211" s="21" t="s">
         <v>690</v>
-      </c>
-      <c r="G211" s="21" t="s">
-        <v>691</v>
       </c>
       <c r="H211" s="9" t="s">
         <v>128</v>
       </c>
       <c r="I211" s="8" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="J211" s="9" t="s">
         <v>394</v>
       </c>
       <c r="K211" s="8" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="212" spans="1:11" ht="20" customHeight="1">
@@ -11466,28 +11539,28 @@
         <v>560</v>
       </c>
       <c r="D212" s="26" t="s">
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E212" s="16" t="s">
         <v>558</v>
       </c>
       <c r="F212" s="21" t="s">
+        <v>692</v>
+      </c>
+      <c r="G212" s="21" t="s">
         <v>693</v>
       </c>
-      <c r="G212" s="21" t="s">
-        <v>694</v>
-      </c>
       <c r="H212" s="9" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I212" s="8" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="J212" s="9" t="s">
         <v>342</v>
       </c>
       <c r="K212" s="8" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="213" spans="1:11" ht="20" customHeight="1">
@@ -11501,28 +11574,28 @@
         <v>560</v>
       </c>
       <c r="D213" s="26" t="s">
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E213" s="16" t="s">
         <v>558</v>
       </c>
       <c r="F213" s="21" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="G213" s="21" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="H213" s="9" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I213" s="8" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="J213" s="9" t="s">
         <v>342</v>
       </c>
       <c r="K213" s="8" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="214" spans="1:11" ht="20" customHeight="1">
@@ -11536,7 +11609,7 @@
         <v>560</v>
       </c>
       <c r="D214" s="26" t="s">
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E214" s="16" t="s">
         <v>558</v>
@@ -11555,7 +11628,7 @@
         <v>342</v>
       </c>
       <c r="K214" s="8" t="s">
-        <v>670</v>
+        <v>797</v>
       </c>
     </row>
     <row r="215" spans="1:11" ht="20" customHeight="1">
@@ -11569,7 +11642,7 @@
         <v>560</v>
       </c>
       <c r="D215" s="26" t="s">
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E215" s="16" t="s">
         <v>558</v>
@@ -11588,7 +11661,7 @@
         <v>342</v>
       </c>
       <c r="K215" s="8" t="s">
-        <v>670</v>
+        <v>797</v>
       </c>
     </row>
     <row r="216" spans="1:11" ht="20" customHeight="1">
@@ -11602,7 +11675,7 @@
         <v>560</v>
       </c>
       <c r="D216" s="26" t="s">
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E216" s="16" t="s">
         <v>558</v>
@@ -11621,7 +11694,7 @@
         <v>342</v>
       </c>
       <c r="K216" s="8" t="s">
-        <v>670</v>
+        <v>797</v>
       </c>
     </row>
     <row r="217" spans="1:11" ht="20" customHeight="1">
@@ -11632,26 +11705,26 @@
         <v>559</v>
       </c>
       <c r="C217" s="9" t="s">
-        <v>566</v>
-      </c>
-      <c r="D217" s="9" t="s">
-        <v>671</v>
+        <v>560</v>
+      </c>
+      <c r="D217" s="26" t="s">
+        <v>777</v>
       </c>
       <c r="E217" s="16" t="s">
         <v>558</v>
       </c>
       <c r="F217" s="21" t="s">
-        <v>672</v>
+        <v>576</v>
       </c>
       <c r="G217" s="21" t="s">
-        <v>673</v>
+        <v>577</v>
       </c>
       <c r="H217" s="9" t="s">
         <v>341</v>
       </c>
       <c r="I217" s="8"/>
       <c r="J217" s="9" t="s">
-        <v>342</v>
+        <v>5</v>
       </c>
       <c r="K217" s="8" t="s">
         <v>619</v>
@@ -11665,25 +11738,25 @@
         <v>559</v>
       </c>
       <c r="C218" s="9" t="s">
-        <v>566</v>
-      </c>
-      <c r="D218" s="9" t="s">
-        <v>671</v>
+        <v>560</v>
+      </c>
+      <c r="D218" s="26" t="s">
+        <v>777</v>
       </c>
       <c r="E218" s="16" t="s">
         <v>558</v>
       </c>
-      <c r="F218" s="21" t="s">
-        <v>578</v>
-      </c>
-      <c r="G218" s="21" t="s">
+      <c r="F218" s="27" t="s">
+        <v>778</v>
+      </c>
+      <c r="G218" s="27" t="s">
         <v>579</v>
       </c>
       <c r="H218" s="9" t="s">
         <v>81</v>
       </c>
       <c r="I218" s="8" t="s">
-        <v>700</v>
+        <v>781</v>
       </c>
       <c r="J218" s="9" t="s">
         <v>394</v>
@@ -11700,10 +11773,10 @@
         <v>559</v>
       </c>
       <c r="C219" s="9" t="s">
-        <v>566</v>
-      </c>
-      <c r="D219" s="9" t="s">
-        <v>671</v>
+        <v>560</v>
+      </c>
+      <c r="D219" s="26" t="s">
+        <v>777</v>
       </c>
       <c r="E219" s="16" t="s">
         <v>558</v>
@@ -11712,19 +11785,19 @@
         <v>581</v>
       </c>
       <c r="G219" s="21" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="H219" s="9" t="s">
         <v>81</v>
       </c>
       <c r="I219" s="8" t="s">
-        <v>700</v>
+        <v>779</v>
       </c>
       <c r="J219" s="9" t="s">
         <v>394</v>
       </c>
       <c r="K219" s="8" t="s">
-        <v>701</v>
+        <v>782</v>
       </c>
     </row>
     <row r="220" spans="1:11" ht="20" customHeight="1">
@@ -11735,10 +11808,10 @@
         <v>559</v>
       </c>
       <c r="C220" s="9" t="s">
-        <v>566</v>
-      </c>
-      <c r="D220" s="9" t="s">
-        <v>671</v>
+        <v>560</v>
+      </c>
+      <c r="D220" s="26" t="s">
+        <v>777</v>
       </c>
       <c r="E220" s="16" t="s">
         <v>558</v>
@@ -11747,19 +11820,19 @@
         <v>584</v>
       </c>
       <c r="G220" s="21" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="H220" s="9" t="s">
         <v>81</v>
       </c>
       <c r="I220" s="8" t="s">
-        <v>700</v>
+        <v>779</v>
       </c>
       <c r="J220" s="9" t="s">
         <v>394</v>
       </c>
       <c r="K220" s="8" t="s">
-        <v>701</v>
+        <v>782</v>
       </c>
     </row>
     <row r="221" spans="1:11" ht="20" customHeight="1">
@@ -11770,31 +11843,31 @@
         <v>559</v>
       </c>
       <c r="C221" s="9" t="s">
-        <v>566</v>
-      </c>
-      <c r="D221" s="9" t="s">
-        <v>671</v>
+        <v>560</v>
+      </c>
+      <c r="D221" s="26" t="s">
+        <v>777</v>
       </c>
       <c r="E221" s="16" t="s">
         <v>558</v>
       </c>
       <c r="F221" s="21" t="s">
-        <v>714</v>
+        <v>783</v>
       </c>
       <c r="G221" s="21" t="s">
-        <v>715</v>
+        <v>784</v>
       </c>
       <c r="H221" s="9" t="s">
-        <v>3</v>
+        <v>626</v>
       </c>
       <c r="I221" s="8" t="s">
-        <v>712</v>
+        <v>780</v>
       </c>
       <c r="J221" s="9" t="s">
         <v>394</v>
       </c>
       <c r="K221" s="8" t="s">
-        <v>625</v>
+        <v>665</v>
       </c>
     </row>
     <row r="222" spans="1:11" ht="20" customHeight="1">
@@ -11805,27 +11878,31 @@
         <v>559</v>
       </c>
       <c r="C222" s="9" t="s">
-        <v>566</v>
-      </c>
-      <c r="D222" s="9" t="s">
-        <v>671</v>
+        <v>560</v>
+      </c>
+      <c r="D222" s="26" t="s">
+        <v>777</v>
       </c>
       <c r="E222" s="16" t="s">
         <v>558</v>
       </c>
       <c r="F222" s="21" t="s">
-        <v>674</v>
+        <v>685</v>
       </c>
       <c r="G222" s="21" t="s">
-        <v>675</v>
-      </c>
-      <c r="H222" s="9"/>
-      <c r="I222" s="8"/>
+        <v>686</v>
+      </c>
+      <c r="H222" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="I222" s="8" t="s">
+        <v>785</v>
+      </c>
       <c r="J222" s="9" t="s">
         <v>394</v>
       </c>
       <c r="K222" s="8" t="s">
-        <v>702</v>
+        <v>708</v>
       </c>
     </row>
     <row r="223" spans="1:11" ht="20" customHeight="1">
@@ -11836,31 +11913,31 @@
         <v>559</v>
       </c>
       <c r="C223" s="9" t="s">
-        <v>566</v>
-      </c>
-      <c r="D223" s="9" t="s">
-        <v>671</v>
+        <v>560</v>
+      </c>
+      <c r="D223" s="26" t="s">
+        <v>777</v>
       </c>
       <c r="E223" s="16" t="s">
         <v>558</v>
       </c>
       <c r="F223" s="21" t="s">
-        <v>676</v>
+        <v>689</v>
       </c>
       <c r="G223" s="21" t="s">
-        <v>677</v>
+        <v>690</v>
       </c>
       <c r="H223" s="9" t="s">
-        <v>393</v>
+        <v>128</v>
       </c>
       <c r="I223" s="8" t="s">
-        <v>703</v>
+        <v>787</v>
       </c>
       <c r="J223" s="9" t="s">
         <v>394</v>
       </c>
       <c r="K223" s="8" t="s">
-        <v>704</v>
+        <v>695</v>
       </c>
     </row>
     <row r="224" spans="1:11" ht="20" customHeight="1">
@@ -11871,31 +11948,31 @@
         <v>559</v>
       </c>
       <c r="C224" s="9" t="s">
-        <v>566</v>
-      </c>
-      <c r="D224" s="9" t="s">
-        <v>671</v>
+        <v>560</v>
+      </c>
+      <c r="D224" s="26" t="s">
+        <v>777</v>
       </c>
       <c r="E224" s="16" t="s">
         <v>558</v>
       </c>
       <c r="F224" s="21" t="s">
-        <v>678</v>
+        <v>786</v>
       </c>
       <c r="G224" s="21" t="s">
-        <v>679</v>
+        <v>789</v>
       </c>
       <c r="H224" s="9" t="s">
-        <v>393</v>
+        <v>698</v>
       </c>
       <c r="I224" s="8" t="s">
-        <v>703</v>
+        <v>697</v>
       </c>
       <c r="J224" s="9" t="s">
-        <v>394</v>
+        <v>342</v>
       </c>
       <c r="K224" s="8" t="s">
-        <v>705</v>
+        <v>788</v>
       </c>
     </row>
     <row r="225" spans="1:11" ht="20" customHeight="1">
@@ -11906,31 +11983,29 @@
         <v>559</v>
       </c>
       <c r="C225" s="9" t="s">
-        <v>566</v>
-      </c>
-      <c r="D225" s="9" t="s">
-        <v>671</v>
+        <v>560</v>
+      </c>
+      <c r="D225" s="26" t="s">
+        <v>777</v>
       </c>
       <c r="E225" s="16" t="s">
         <v>558</v>
       </c>
       <c r="F225" s="21" t="s">
-        <v>680</v>
+        <v>790</v>
       </c>
       <c r="G225" s="21" t="s">
-        <v>681</v>
+        <v>791</v>
       </c>
       <c r="H225" s="9" t="s">
-        <v>393</v>
-      </c>
-      <c r="I225" s="8" t="s">
-        <v>703</v>
-      </c>
+        <v>669</v>
+      </c>
+      <c r="I225" s="8"/>
       <c r="J225" s="9" t="s">
-        <v>394</v>
+        <v>342</v>
       </c>
       <c r="K225" s="8" t="s">
-        <v>705</v>
+        <v>796</v>
       </c>
     </row>
     <row r="226" spans="1:11" ht="20" customHeight="1">
@@ -11941,31 +12016,29 @@
         <v>559</v>
       </c>
       <c r="C226" s="9" t="s">
-        <v>566</v>
-      </c>
-      <c r="D226" s="9" t="s">
-        <v>671</v>
+        <v>560</v>
+      </c>
+      <c r="D226" s="26" t="s">
+        <v>777</v>
       </c>
       <c r="E226" s="16" t="s">
         <v>558</v>
       </c>
-      <c r="F226" s="21" t="s">
-        <v>682</v>
-      </c>
-      <c r="G226" s="21" t="s">
-        <v>683</v>
+      <c r="F226" s="27" t="s">
+        <v>792</v>
+      </c>
+      <c r="G226" s="27" t="s">
+        <v>793</v>
       </c>
       <c r="H226" s="9" t="s">
-        <v>393</v>
-      </c>
-      <c r="I226" s="8" t="s">
-        <v>703</v>
-      </c>
+        <v>798</v>
+      </c>
+      <c r="I226" s="8"/>
       <c r="J226" s="9" t="s">
-        <v>394</v>
+        <v>342</v>
       </c>
       <c r="K226" s="8" t="s">
-        <v>705</v>
+        <v>796</v>
       </c>
     </row>
     <row r="227" spans="1:11" ht="20" customHeight="1">
@@ -11976,31 +12049,29 @@
         <v>559</v>
       </c>
       <c r="C227" s="9" t="s">
-        <v>566</v>
-      </c>
-      <c r="D227" s="9" t="s">
-        <v>671</v>
+        <v>560</v>
+      </c>
+      <c r="D227" s="26" t="s">
+        <v>777</v>
       </c>
       <c r="E227" s="16" t="s">
         <v>558</v>
       </c>
-      <c r="F227" s="21" t="s">
-        <v>615</v>
-      </c>
-      <c r="G227" s="21" t="s">
-        <v>616</v>
+      <c r="F227" s="27" t="s">
+        <v>794</v>
+      </c>
+      <c r="G227" s="27" t="s">
+        <v>795</v>
       </c>
       <c r="H227" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="I227" s="8" t="s">
-        <v>706</v>
-      </c>
+        <v>669</v>
+      </c>
+      <c r="I227" s="8"/>
       <c r="J227" s="9" t="s">
-        <v>394</v>
+        <v>342</v>
       </c>
       <c r="K227" s="8" t="s">
-        <v>663</v>
+        <v>796</v>
       </c>
     </row>
     <row r="228" spans="1:11" ht="20" customHeight="1">
@@ -12014,28 +12085,26 @@
         <v>566</v>
       </c>
       <c r="D228" s="9" t="s">
+        <v>670</v>
+      </c>
+      <c r="E228" s="16" t="s">
+        <v>558</v>
+      </c>
+      <c r="F228" s="21" t="s">
         <v>671</v>
       </c>
-      <c r="E228" s="16" t="s">
-        <v>558</v>
-      </c>
-      <c r="F228" s="21" t="s">
-        <v>617</v>
-      </c>
       <c r="G228" s="21" t="s">
-        <v>618</v>
+        <v>672</v>
       </c>
       <c r="H228" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="I228" s="8" t="s">
-        <v>711</v>
-      </c>
+        <v>341</v>
+      </c>
+      <c r="I228" s="8"/>
       <c r="J228" s="9" t="s">
-        <v>394</v>
+        <v>342</v>
       </c>
       <c r="K228" s="8" t="s">
-        <v>665</v>
+        <v>619</v>
       </c>
     </row>
     <row r="229" spans="1:11" ht="20" customHeight="1">
@@ -12049,28 +12118,28 @@
         <v>566</v>
       </c>
       <c r="D229" s="9" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="E229" s="16" t="s">
         <v>558</v>
       </c>
       <c r="F229" s="21" t="s">
-        <v>684</v>
+        <v>578</v>
       </c>
       <c r="G229" s="21" t="s">
-        <v>685</v>
+        <v>579</v>
       </c>
       <c r="H229" s="9" t="s">
-        <v>668</v>
+        <v>81</v>
       </c>
       <c r="I229" s="8" t="s">
-        <v>707</v>
+        <v>699</v>
       </c>
       <c r="J229" s="9" t="s">
         <v>394</v>
       </c>
       <c r="K229" s="8" t="s">
-        <v>666</v>
+        <v>621</v>
       </c>
     </row>
     <row r="230" spans="1:11" ht="20" customHeight="1">
@@ -12084,28 +12153,28 @@
         <v>566</v>
       </c>
       <c r="D230" s="9" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="E230" s="16" t="s">
         <v>558</v>
       </c>
       <c r="F230" s="21" t="s">
-        <v>686</v>
+        <v>581</v>
       </c>
       <c r="G230" s="21" t="s">
-        <v>687</v>
+        <v>582</v>
       </c>
       <c r="H230" s="9" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="I230" s="8" t="s">
-        <v>710</v>
+        <v>699</v>
       </c>
       <c r="J230" s="9" t="s">
         <v>394</v>
       </c>
       <c r="K230" s="8" t="s">
-        <v>709</v>
+        <v>700</v>
       </c>
     </row>
     <row r="231" spans="1:11" ht="20" customHeight="1">
@@ -12119,28 +12188,28 @@
         <v>566</v>
       </c>
       <c r="D231" s="9" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="E231" s="16" t="s">
         <v>558</v>
       </c>
       <c r="F231" s="21" t="s">
-        <v>690</v>
+        <v>584</v>
       </c>
       <c r="G231" s="21" t="s">
-        <v>691</v>
+        <v>585</v>
       </c>
       <c r="H231" s="9" t="s">
-        <v>128</v>
+        <v>81</v>
       </c>
       <c r="I231" s="8" t="s">
-        <v>718</v>
+        <v>699</v>
       </c>
       <c r="J231" s="9" t="s">
         <v>394</v>
       </c>
       <c r="K231" s="8" t="s">
-        <v>696</v>
+        <v>700</v>
       </c>
     </row>
     <row r="232" spans="1:11" ht="20" customHeight="1">
@@ -12154,28 +12223,28 @@
         <v>566</v>
       </c>
       <c r="D232" s="9" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="E232" s="16" t="s">
         <v>558</v>
       </c>
       <c r="F232" s="21" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
       <c r="G232" s="21" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="H232" s="9" t="s">
-        <v>699</v>
+        <v>3</v>
       </c>
       <c r="I232" s="8" t="s">
-        <v>698</v>
+        <v>711</v>
       </c>
       <c r="J232" s="9" t="s">
-        <v>342</v>
+        <v>394</v>
       </c>
       <c r="K232" s="8" t="s">
-        <v>719</v>
+        <v>625</v>
       </c>
     </row>
     <row r="233" spans="1:11" ht="20" customHeight="1">
@@ -12189,28 +12258,24 @@
         <v>566</v>
       </c>
       <c r="D233" s="9" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="E233" s="16" t="s">
         <v>558</v>
       </c>
       <c r="F233" s="21" t="s">
-        <v>692</v>
+        <v>673</v>
       </c>
       <c r="G233" s="21" t="s">
-        <v>776</v>
-      </c>
-      <c r="H233" s="9" t="s">
-        <v>699</v>
-      </c>
-      <c r="I233" s="8" t="s">
-        <v>698</v>
-      </c>
+        <v>674</v>
+      </c>
+      <c r="H233" s="9"/>
+      <c r="I233" s="8"/>
       <c r="J233" s="9" t="s">
-        <v>342</v>
+        <v>394</v>
       </c>
       <c r="K233" s="8" t="s">
-        <v>719</v>
+        <v>701</v>
       </c>
     </row>
     <row r="234" spans="1:11" ht="20" customHeight="1">
@@ -12224,26 +12289,28 @@
         <v>566</v>
       </c>
       <c r="D234" s="9" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="E234" s="16" t="s">
         <v>558</v>
       </c>
       <c r="F234" s="21" t="s">
-        <v>671</v>
+        <v>675</v>
       </c>
       <c r="G234" s="21" t="s">
-        <v>573</v>
+        <v>676</v>
       </c>
       <c r="H234" s="9" t="s">
-        <v>669</v>
-      </c>
-      <c r="I234" s="8"/>
+        <v>393</v>
+      </c>
+      <c r="I234" s="8" t="s">
+        <v>702</v>
+      </c>
       <c r="J234" s="9" t="s">
-        <v>342</v>
+        <v>394</v>
       </c>
       <c r="K234" s="8" t="s">
-        <v>713</v>
+        <v>703</v>
       </c>
     </row>
     <row r="235" spans="1:11" ht="20" customHeight="1">
@@ -12257,26 +12324,28 @@
         <v>566</v>
       </c>
       <c r="D235" s="9" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="E235" s="16" t="s">
         <v>558</v>
       </c>
       <c r="F235" s="21" t="s">
-        <v>688</v>
+        <v>677</v>
       </c>
       <c r="G235" s="21" t="s">
-        <v>689</v>
+        <v>678</v>
       </c>
       <c r="H235" s="9" t="s">
-        <v>669</v>
-      </c>
-      <c r="I235" s="8"/>
+        <v>393</v>
+      </c>
+      <c r="I235" s="8" t="s">
+        <v>702</v>
+      </c>
       <c r="J235" s="9" t="s">
-        <v>342</v>
+        <v>394</v>
       </c>
       <c r="K235" s="8" t="s">
-        <v>713</v>
+        <v>704</v>
       </c>
     </row>
     <row r="236" spans="1:11" ht="20" customHeight="1">
@@ -12290,26 +12359,28 @@
         <v>566</v>
       </c>
       <c r="D236" s="9" t="s">
-        <v>574</v>
+        <v>670</v>
       </c>
       <c r="E236" s="16" t="s">
         <v>558</v>
       </c>
       <c r="F236" s="21" t="s">
-        <v>720</v>
+        <v>679</v>
       </c>
       <c r="G236" s="21" t="s">
-        <v>721</v>
+        <v>680</v>
       </c>
       <c r="H236" s="9" t="s">
-        <v>341</v>
-      </c>
-      <c r="I236" s="8"/>
+        <v>393</v>
+      </c>
+      <c r="I236" s="8" t="s">
+        <v>702</v>
+      </c>
       <c r="J236" s="9" t="s">
-        <v>342</v>
+        <v>394</v>
       </c>
       <c r="K236" s="8" t="s">
-        <v>619</v>
+        <v>704</v>
       </c>
     </row>
     <row r="237" spans="1:11" ht="20" customHeight="1">
@@ -12323,28 +12394,28 @@
         <v>566</v>
       </c>
       <c r="D237" s="9" t="s">
-        <v>574</v>
+        <v>670</v>
       </c>
       <c r="E237" s="16" t="s">
         <v>558</v>
       </c>
       <c r="F237" s="21" t="s">
-        <v>722</v>
+        <v>681</v>
       </c>
       <c r="G237" s="21" t="s">
-        <v>723</v>
+        <v>682</v>
       </c>
       <c r="H237" s="9" t="s">
         <v>393</v>
       </c>
       <c r="I237" s="8" t="s">
-        <v>725</v>
+        <v>702</v>
       </c>
       <c r="J237" s="9" t="s">
         <v>394</v>
       </c>
       <c r="K237" s="8" t="s">
-        <v>625</v>
+        <v>704</v>
       </c>
     </row>
     <row r="238" spans="1:11" ht="20" customHeight="1">
@@ -12358,28 +12429,28 @@
         <v>566</v>
       </c>
       <c r="D238" s="9" t="s">
-        <v>574</v>
+        <v>670</v>
       </c>
       <c r="E238" s="16" t="s">
         <v>558</v>
       </c>
       <c r="F238" s="21" t="s">
-        <v>676</v>
+        <v>615</v>
       </c>
       <c r="G238" s="21" t="s">
-        <v>724</v>
+        <v>616</v>
       </c>
       <c r="H238" s="9" t="s">
-        <v>393</v>
+        <v>70</v>
       </c>
       <c r="I238" s="8" t="s">
-        <v>727</v>
+        <v>705</v>
       </c>
       <c r="J238" s="9" t="s">
         <v>394</v>
       </c>
       <c r="K238" s="8" t="s">
-        <v>704</v>
+        <v>663</v>
       </c>
     </row>
     <row r="239" spans="1:11" ht="20" customHeight="1">
@@ -12393,28 +12464,28 @@
         <v>566</v>
       </c>
       <c r="D239" s="9" t="s">
-        <v>574</v>
+        <v>670</v>
       </c>
       <c r="E239" s="16" t="s">
         <v>558</v>
       </c>
       <c r="F239" s="21" t="s">
-        <v>678</v>
+        <v>617</v>
       </c>
       <c r="G239" s="21" t="s">
-        <v>679</v>
+        <v>618</v>
       </c>
       <c r="H239" s="9" t="s">
-        <v>393</v>
+        <v>3</v>
       </c>
       <c r="I239" s="8" t="s">
-        <v>726</v>
+        <v>710</v>
       </c>
       <c r="J239" s="9" t="s">
         <v>394</v>
       </c>
       <c r="K239" s="8" t="s">
-        <v>728</v>
+        <v>665</v>
       </c>
     </row>
     <row r="240" spans="1:11" ht="20" customHeight="1">
@@ -12428,28 +12499,28 @@
         <v>566</v>
       </c>
       <c r="D240" s="9" t="s">
-        <v>574</v>
+        <v>670</v>
       </c>
       <c r="E240" s="16" t="s">
         <v>558</v>
       </c>
       <c r="F240" s="21" t="s">
-        <v>680</v>
+        <v>683</v>
       </c>
       <c r="G240" s="21" t="s">
-        <v>681</v>
+        <v>684</v>
       </c>
       <c r="H240" s="9" t="s">
-        <v>393</v>
+        <v>668</v>
       </c>
       <c r="I240" s="8" t="s">
-        <v>726</v>
+        <v>706</v>
       </c>
       <c r="J240" s="9" t="s">
         <v>394</v>
       </c>
       <c r="K240" s="8" t="s">
-        <v>728</v>
+        <v>666</v>
       </c>
     </row>
     <row r="241" spans="1:11" ht="20" customHeight="1">
@@ -12463,28 +12534,28 @@
         <v>566</v>
       </c>
       <c r="D241" s="9" t="s">
-        <v>574</v>
+        <v>670</v>
       </c>
       <c r="E241" s="16" t="s">
         <v>558</v>
       </c>
       <c r="F241" s="21" t="s">
-        <v>682</v>
+        <v>685</v>
       </c>
       <c r="G241" s="21" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="H241" s="9" t="s">
-        <v>393</v>
+        <v>70</v>
       </c>
       <c r="I241" s="8" t="s">
-        <v>726</v>
+        <v>709</v>
       </c>
       <c r="J241" s="9" t="s">
         <v>394</v>
       </c>
       <c r="K241" s="8" t="s">
-        <v>728</v>
+        <v>708</v>
       </c>
     </row>
     <row r="242" spans="1:11" ht="20" customHeight="1">
@@ -12498,28 +12569,28 @@
         <v>566</v>
       </c>
       <c r="D242" s="9" t="s">
-        <v>574</v>
+        <v>670</v>
       </c>
       <c r="E242" s="16" t="s">
         <v>558</v>
       </c>
       <c r="F242" s="21" t="s">
-        <v>733</v>
+        <v>689</v>
       </c>
       <c r="G242" s="21" t="s">
-        <v>734</v>
+        <v>690</v>
       </c>
       <c r="H242" s="9" t="s">
-        <v>393</v>
+        <v>128</v>
       </c>
       <c r="I242" s="8" t="s">
-        <v>731</v>
+        <v>717</v>
       </c>
       <c r="J242" s="9" t="s">
         <v>394</v>
       </c>
       <c r="K242" s="8" t="s">
-        <v>729</v>
+        <v>695</v>
       </c>
     </row>
     <row r="243" spans="1:11" ht="20" customHeight="1">
@@ -12533,28 +12604,28 @@
         <v>566</v>
       </c>
       <c r="D243" s="9" t="s">
-        <v>574</v>
+        <v>670</v>
       </c>
       <c r="E243" s="16" t="s">
         <v>558</v>
       </c>
       <c r="F243" s="21" t="s">
-        <v>735</v>
+        <v>715</v>
       </c>
       <c r="G243" s="21" t="s">
-        <v>736</v>
+        <v>716</v>
       </c>
       <c r="H243" s="9" t="s">
-        <v>393</v>
+        <v>698</v>
       </c>
       <c r="I243" s="8" t="s">
-        <v>730</v>
+        <v>697</v>
       </c>
       <c r="J243" s="9" t="s">
-        <v>394</v>
+        <v>342</v>
       </c>
       <c r="K243" s="8" t="s">
-        <v>732</v>
+        <v>718</v>
       </c>
     </row>
     <row r="244" spans="1:11" ht="20" customHeight="1">
@@ -12568,28 +12639,28 @@
         <v>566</v>
       </c>
       <c r="D244" s="9" t="s">
-        <v>574</v>
+        <v>670</v>
       </c>
       <c r="E244" s="16" t="s">
         <v>558</v>
       </c>
       <c r="F244" s="21" t="s">
-        <v>737</v>
+        <v>691</v>
       </c>
       <c r="G244" s="21" t="s">
-        <v>738</v>
+        <v>775</v>
       </c>
       <c r="H244" s="9" t="s">
-        <v>393</v>
+        <v>698</v>
       </c>
       <c r="I244" s="8" t="s">
-        <v>730</v>
+        <v>697</v>
       </c>
       <c r="J244" s="9" t="s">
-        <v>394</v>
+        <v>342</v>
       </c>
       <c r="K244" s="8" t="s">
-        <v>732</v>
+        <v>718</v>
       </c>
     </row>
     <row r="245" spans="1:11" ht="20" customHeight="1">
@@ -12603,28 +12674,26 @@
         <v>566</v>
       </c>
       <c r="D245" s="9" t="s">
-        <v>574</v>
+        <v>670</v>
       </c>
       <c r="E245" s="16" t="s">
         <v>558</v>
       </c>
       <c r="F245" s="21" t="s">
-        <v>739</v>
+        <v>670</v>
       </c>
       <c r="G245" s="21" t="s">
-        <v>740</v>
+        <v>573</v>
       </c>
       <c r="H245" s="9" t="s">
-        <v>393</v>
-      </c>
-      <c r="I245" s="8" t="s">
-        <v>730</v>
-      </c>
+        <v>669</v>
+      </c>
+      <c r="I245" s="8"/>
       <c r="J245" s="9" t="s">
-        <v>394</v>
+        <v>342</v>
       </c>
       <c r="K245" s="8" t="s">
-        <v>732</v>
+        <v>712</v>
       </c>
     </row>
     <row r="246" spans="1:11" ht="20" customHeight="1">
@@ -12638,28 +12707,26 @@
         <v>566</v>
       </c>
       <c r="D246" s="9" t="s">
-        <v>574</v>
+        <v>670</v>
       </c>
       <c r="E246" s="16" t="s">
         <v>558</v>
       </c>
       <c r="F246" s="21" t="s">
-        <v>615</v>
+        <v>687</v>
       </c>
       <c r="G246" s="21" t="s">
-        <v>616</v>
+        <v>688</v>
       </c>
       <c r="H246" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="I246" s="8" t="s">
-        <v>741</v>
-      </c>
+        <v>669</v>
+      </c>
+      <c r="I246" s="8"/>
       <c r="J246" s="9" t="s">
-        <v>394</v>
+        <v>342</v>
       </c>
       <c r="K246" s="8" t="s">
-        <v>663</v>
+        <v>712</v>
       </c>
     </row>
     <row r="247" spans="1:11" ht="20" customHeight="1">
@@ -12679,22 +12746,20 @@
         <v>558</v>
       </c>
       <c r="F247" s="21" t="s">
-        <v>617</v>
+        <v>719</v>
       </c>
       <c r="G247" s="21" t="s">
-        <v>618</v>
+        <v>720</v>
       </c>
       <c r="H247" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="I247" s="8" t="s">
-        <v>742</v>
-      </c>
+        <v>341</v>
+      </c>
+      <c r="I247" s="8"/>
       <c r="J247" s="9" t="s">
-        <v>394</v>
+        <v>342</v>
       </c>
       <c r="K247" s="8" t="s">
-        <v>665</v>
+        <v>619</v>
       </c>
     </row>
     <row r="248" spans="1:11" ht="20" customHeight="1">
@@ -12714,22 +12779,22 @@
         <v>558</v>
       </c>
       <c r="F248" s="21" t="s">
-        <v>686</v>
+        <v>721</v>
       </c>
       <c r="G248" s="21" t="s">
-        <v>687</v>
+        <v>722</v>
       </c>
       <c r="H248" s="9" t="s">
-        <v>70</v>
+        <v>393</v>
       </c>
       <c r="I248" s="8" t="s">
-        <v>743</v>
+        <v>724</v>
       </c>
       <c r="J248" s="9" t="s">
         <v>394</v>
       </c>
       <c r="K248" s="8" t="s">
-        <v>709</v>
+        <v>625</v>
       </c>
     </row>
     <row r="249" spans="1:11" ht="20" customHeight="1">
@@ -12749,22 +12814,22 @@
         <v>558</v>
       </c>
       <c r="F249" s="21" t="s">
-        <v>690</v>
+        <v>675</v>
       </c>
       <c r="G249" s="21" t="s">
-        <v>691</v>
+        <v>723</v>
       </c>
       <c r="H249" s="9" t="s">
-        <v>128</v>
+        <v>393</v>
       </c>
       <c r="I249" s="8" t="s">
-        <v>746</v>
+        <v>726</v>
       </c>
       <c r="J249" s="9" t="s">
         <v>394</v>
       </c>
       <c r="K249" s="8" t="s">
-        <v>696</v>
+        <v>703</v>
       </c>
     </row>
     <row r="250" spans="1:11" ht="20" customHeight="1">
@@ -12784,22 +12849,22 @@
         <v>558</v>
       </c>
       <c r="F250" s="21" t="s">
-        <v>744</v>
+        <v>677</v>
       </c>
       <c r="G250" s="21" t="s">
-        <v>745</v>
+        <v>678</v>
       </c>
       <c r="H250" s="9" t="s">
-        <v>699</v>
+        <v>393</v>
       </c>
       <c r="I250" s="8" t="s">
-        <v>698</v>
+        <v>725</v>
       </c>
       <c r="J250" s="9" t="s">
-        <v>342</v>
+        <v>394</v>
       </c>
       <c r="K250" s="8" t="s">
-        <v>747</v>
+        <v>727</v>
       </c>
     </row>
     <row r="251" spans="1:11" ht="20" customHeight="1">
@@ -12819,22 +12884,22 @@
         <v>558</v>
       </c>
       <c r="F251" s="21" t="s">
-        <v>692</v>
+        <v>679</v>
       </c>
       <c r="G251" s="21" t="s">
-        <v>776</v>
+        <v>680</v>
       </c>
       <c r="H251" s="9" t="s">
-        <v>699</v>
+        <v>393</v>
       </c>
       <c r="I251" s="8" t="s">
-        <v>698</v>
+        <v>725</v>
       </c>
       <c r="J251" s="9" t="s">
-        <v>342</v>
+        <v>394</v>
       </c>
       <c r="K251" s="8" t="s">
-        <v>747</v>
+        <v>727</v>
       </c>
     </row>
     <row r="252" spans="1:11" ht="20" customHeight="1">
@@ -12854,20 +12919,22 @@
         <v>558</v>
       </c>
       <c r="F252" s="21" t="s">
-        <v>748</v>
+        <v>681</v>
       </c>
       <c r="G252" s="21" t="s">
-        <v>749</v>
+        <v>682</v>
       </c>
       <c r="H252" s="9" t="s">
-        <v>763</v>
-      </c>
-      <c r="I252" s="8"/>
+        <v>393</v>
+      </c>
+      <c r="I252" s="8" t="s">
+        <v>725</v>
+      </c>
       <c r="J252" s="9" t="s">
-        <v>342</v>
+        <v>394</v>
       </c>
       <c r="K252" s="8" t="s">
-        <v>762</v>
+        <v>727</v>
       </c>
     </row>
     <row r="253" spans="1:11" ht="20" customHeight="1">
@@ -12887,20 +12954,22 @@
         <v>558</v>
       </c>
       <c r="F253" s="21" t="s">
-        <v>750</v>
+        <v>732</v>
       </c>
       <c r="G253" s="21" t="s">
-        <v>751</v>
+        <v>733</v>
       </c>
       <c r="H253" s="9" t="s">
-        <v>763</v>
-      </c>
-      <c r="I253" s="8"/>
+        <v>393</v>
+      </c>
+      <c r="I253" s="8" t="s">
+        <v>730</v>
+      </c>
       <c r="J253" s="9" t="s">
-        <v>342</v>
+        <v>394</v>
       </c>
       <c r="K253" s="8" t="s">
-        <v>762</v>
+        <v>728</v>
       </c>
     </row>
     <row r="254" spans="1:11" ht="20" customHeight="1">
@@ -12920,20 +12989,22 @@
         <v>558</v>
       </c>
       <c r="F254" s="21" t="s">
-        <v>752</v>
+        <v>734</v>
       </c>
       <c r="G254" s="21" t="s">
-        <v>753</v>
+        <v>735</v>
       </c>
       <c r="H254" s="9" t="s">
-        <v>763</v>
-      </c>
-      <c r="I254" s="8"/>
+        <v>393</v>
+      </c>
+      <c r="I254" s="8" t="s">
+        <v>729</v>
+      </c>
       <c r="J254" s="9" t="s">
-        <v>342</v>
+        <v>394</v>
       </c>
       <c r="K254" s="8" t="s">
-        <v>762</v>
+        <v>731</v>
       </c>
     </row>
     <row r="255" spans="1:11" ht="20" customHeight="1">
@@ -12953,20 +13024,22 @@
         <v>558</v>
       </c>
       <c r="F255" s="21" t="s">
-        <v>754</v>
+        <v>736</v>
       </c>
       <c r="G255" s="21" t="s">
-        <v>755</v>
+        <v>737</v>
       </c>
       <c r="H255" s="9" t="s">
-        <v>763</v>
-      </c>
-      <c r="I255" s="8"/>
+        <v>393</v>
+      </c>
+      <c r="I255" s="8" t="s">
+        <v>729</v>
+      </c>
       <c r="J255" s="9" t="s">
-        <v>342</v>
+        <v>394</v>
       </c>
       <c r="K255" s="8" t="s">
-        <v>762</v>
+        <v>731</v>
       </c>
     </row>
     <row r="256" spans="1:11" ht="20" customHeight="1">
@@ -12986,20 +13059,22 @@
         <v>558</v>
       </c>
       <c r="F256" s="21" t="s">
-        <v>756</v>
+        <v>738</v>
       </c>
       <c r="G256" s="21" t="s">
-        <v>757</v>
+        <v>739</v>
       </c>
       <c r="H256" s="9" t="s">
-        <v>763</v>
-      </c>
-      <c r="I256" s="8"/>
+        <v>393</v>
+      </c>
+      <c r="I256" s="8" t="s">
+        <v>729</v>
+      </c>
       <c r="J256" s="9" t="s">
-        <v>342</v>
+        <v>394</v>
       </c>
       <c r="K256" s="8" t="s">
-        <v>762</v>
+        <v>731</v>
       </c>
     </row>
     <row r="257" spans="1:11" ht="20" customHeight="1">
@@ -13019,20 +13094,22 @@
         <v>558</v>
       </c>
       <c r="F257" s="21" t="s">
-        <v>758</v>
+        <v>615</v>
       </c>
       <c r="G257" s="21" t="s">
-        <v>759</v>
+        <v>616</v>
       </c>
       <c r="H257" s="9" t="s">
-        <v>763</v>
-      </c>
-      <c r="I257" s="8"/>
+        <v>70</v>
+      </c>
+      <c r="I257" s="8" t="s">
+        <v>740</v>
+      </c>
       <c r="J257" s="9" t="s">
-        <v>342</v>
+        <v>394</v>
       </c>
       <c r="K257" s="8" t="s">
-        <v>762</v>
+        <v>663</v>
       </c>
     </row>
     <row r="258" spans="1:11" ht="20" customHeight="1">
@@ -13052,20 +13129,22 @@
         <v>558</v>
       </c>
       <c r="F258" s="21" t="s">
-        <v>760</v>
+        <v>617</v>
       </c>
       <c r="G258" s="21" t="s">
-        <v>761</v>
+        <v>618</v>
       </c>
       <c r="H258" s="9" t="s">
-        <v>763</v>
-      </c>
-      <c r="I258" s="8"/>
+        <v>3</v>
+      </c>
+      <c r="I258" s="8" t="s">
+        <v>741</v>
+      </c>
       <c r="J258" s="9" t="s">
-        <v>342</v>
+        <v>394</v>
       </c>
       <c r="K258" s="8" t="s">
-        <v>762</v>
+        <v>665</v>
       </c>
     </row>
     <row r="259" spans="1:11" ht="20" customHeight="1">
@@ -13085,20 +13164,22 @@
         <v>558</v>
       </c>
       <c r="F259" s="21" t="s">
-        <v>764</v>
+        <v>685</v>
       </c>
       <c r="G259" s="21" t="s">
-        <v>765</v>
+        <v>686</v>
       </c>
       <c r="H259" s="9" t="s">
-        <v>766</v>
-      </c>
-      <c r="I259" s="8"/>
+        <v>70</v>
+      </c>
+      <c r="I259" s="8" t="s">
+        <v>742</v>
+      </c>
       <c r="J259" s="9" t="s">
-        <v>342</v>
+        <v>394</v>
       </c>
       <c r="K259" s="8" t="s">
-        <v>773</v>
+        <v>708</v>
       </c>
     </row>
     <row r="260" spans="1:11" ht="20" customHeight="1">
@@ -13118,20 +13199,22 @@
         <v>558</v>
       </c>
       <c r="F260" s="21" t="s">
-        <v>767</v>
+        <v>689</v>
       </c>
       <c r="G260" s="21" t="s">
-        <v>768</v>
+        <v>690</v>
       </c>
       <c r="H260" s="9" t="s">
-        <v>669</v>
-      </c>
-      <c r="I260" s="8"/>
+        <v>128</v>
+      </c>
+      <c r="I260" s="8" t="s">
+        <v>745</v>
+      </c>
       <c r="J260" s="9" t="s">
-        <v>342</v>
+        <v>394</v>
       </c>
       <c r="K260" s="8" t="s">
-        <v>713</v>
+        <v>695</v>
       </c>
     </row>
     <row r="261" spans="1:11" ht="20" customHeight="1">
@@ -13151,18 +13234,22 @@
         <v>558</v>
       </c>
       <c r="F261" s="21" t="s">
-        <v>769</v>
+        <v>743</v>
       </c>
       <c r="G261" s="21" t="s">
-        <v>770</v>
-      </c>
-      <c r="H261" s="9"/>
-      <c r="I261" s="8"/>
+        <v>744</v>
+      </c>
+      <c r="H261" s="9" t="s">
+        <v>698</v>
+      </c>
+      <c r="I261" s="8" t="s">
+        <v>697</v>
+      </c>
       <c r="J261" s="9" t="s">
         <v>342</v>
       </c>
       <c r="K261" s="8" t="s">
-        <v>774</v>
+        <v>746</v>
       </c>
     </row>
     <row r="262" spans="1:11" ht="20" customHeight="1">
@@ -13182,18 +13269,22 @@
         <v>558</v>
       </c>
       <c r="F262" s="21" t="s">
-        <v>771</v>
+        <v>691</v>
       </c>
       <c r="G262" s="21" t="s">
-        <v>772</v>
-      </c>
-      <c r="H262" s="9"/>
-      <c r="I262" s="8"/>
+        <v>775</v>
+      </c>
+      <c r="H262" s="9" t="s">
+        <v>698</v>
+      </c>
+      <c r="I262" s="8" t="s">
+        <v>697</v>
+      </c>
       <c r="J262" s="9" t="s">
         <v>342</v>
       </c>
       <c r="K262" s="8" t="s">
-        <v>775</v>
+        <v>746</v>
       </c>
     </row>
     <row r="263" spans="1:11" ht="20" customHeight="1">
@@ -13201,32 +13292,32 @@
         <v>255</v>
       </c>
       <c r="B263" s="7" t="s">
-        <v>374</v>
+        <v>559</v>
       </c>
       <c r="C263" s="9" t="s">
-        <v>375</v>
-      </c>
-      <c r="D263" s="17" t="s">
-        <v>558</v>
-      </c>
-      <c r="E263" s="17" t="s">
+        <v>566</v>
+      </c>
+      <c r="D263" s="9" t="s">
+        <v>574</v>
+      </c>
+      <c r="E263" s="16" t="s">
         <v>558</v>
       </c>
       <c r="F263" s="21" t="s">
-        <v>381</v>
+        <v>747</v>
       </c>
       <c r="G263" s="21" t="s">
-        <v>378</v>
-      </c>
-      <c r="H263" s="9"/>
-      <c r="I263" s="8" t="s">
-        <v>376</v>
-      </c>
+        <v>748</v>
+      </c>
+      <c r="H263" s="9" t="s">
+        <v>762</v>
+      </c>
+      <c r="I263" s="8"/>
       <c r="J263" s="9" t="s">
         <v>342</v>
       </c>
       <c r="K263" s="8" t="s">
-        <v>375</v>
+        <v>761</v>
       </c>
     </row>
     <row r="264" spans="1:11" ht="20" customHeight="1">
@@ -13234,32 +13325,32 @@
         <v>256</v>
       </c>
       <c r="B264" s="7" t="s">
-        <v>374</v>
+        <v>559</v>
       </c>
       <c r="C264" s="9" t="s">
-        <v>375</v>
-      </c>
-      <c r="D264" s="17" t="s">
-        <v>558</v>
-      </c>
-      <c r="E264" s="17" t="s">
+        <v>566</v>
+      </c>
+      <c r="D264" s="9" t="s">
+        <v>574</v>
+      </c>
+      <c r="E264" s="16" t="s">
         <v>558</v>
       </c>
       <c r="F264" s="21" t="s">
-        <v>382</v>
+        <v>749</v>
       </c>
       <c r="G264" s="21" t="s">
-        <v>379</v>
-      </c>
-      <c r="H264" s="9"/>
-      <c r="I264" s="8" t="s">
-        <v>376</v>
-      </c>
+        <v>750</v>
+      </c>
+      <c r="H264" s="9" t="s">
+        <v>762</v>
+      </c>
+      <c r="I264" s="8"/>
       <c r="J264" s="9" t="s">
         <v>342</v>
       </c>
       <c r="K264" s="8" t="s">
-        <v>375</v>
+        <v>761</v>
       </c>
     </row>
     <row r="265" spans="1:11" ht="20" customHeight="1">
@@ -13267,32 +13358,32 @@
         <v>257</v>
       </c>
       <c r="B265" s="7" t="s">
-        <v>374</v>
+        <v>559</v>
       </c>
       <c r="C265" s="9" t="s">
-        <v>375</v>
-      </c>
-      <c r="D265" s="17" t="s">
-        <v>558</v>
-      </c>
-      <c r="E265" s="17" t="s">
+        <v>566</v>
+      </c>
+      <c r="D265" s="9" t="s">
+        <v>574</v>
+      </c>
+      <c r="E265" s="16" t="s">
         <v>558</v>
       </c>
       <c r="F265" s="21" t="s">
-        <v>377</v>
+        <v>751</v>
       </c>
       <c r="G265" s="21" t="s">
-        <v>380</v>
-      </c>
-      <c r="H265" s="9"/>
-      <c r="I265" s="8" t="s">
-        <v>376</v>
-      </c>
+        <v>752</v>
+      </c>
+      <c r="H265" s="9" t="s">
+        <v>762</v>
+      </c>
+      <c r="I265" s="8"/>
       <c r="J265" s="9" t="s">
         <v>342</v>
       </c>
       <c r="K265" s="8" t="s">
-        <v>375</v>
+        <v>761</v>
       </c>
     </row>
     <row r="266" spans="1:11" ht="20" customHeight="1">
@@ -13300,32 +13391,32 @@
         <v>258</v>
       </c>
       <c r="B266" s="7" t="s">
-        <v>374</v>
+        <v>559</v>
       </c>
       <c r="C266" s="9" t="s">
-        <v>375</v>
-      </c>
-      <c r="D266" s="17" t="s">
-        <v>558</v>
-      </c>
-      <c r="E266" s="17" t="s">
+        <v>566</v>
+      </c>
+      <c r="D266" s="9" t="s">
+        <v>574</v>
+      </c>
+      <c r="E266" s="16" t="s">
         <v>558</v>
       </c>
       <c r="F266" s="21" t="s">
-        <v>384</v>
+        <v>753</v>
       </c>
       <c r="G266" s="21" t="s">
-        <v>385</v>
-      </c>
-      <c r="H266" s="9"/>
-      <c r="I266" s="8" t="s">
-        <v>376</v>
-      </c>
+        <v>754</v>
+      </c>
+      <c r="H266" s="9" t="s">
+        <v>762</v>
+      </c>
+      <c r="I266" s="8"/>
       <c r="J266" s="9" t="s">
         <v>342</v>
       </c>
       <c r="K266" s="8" t="s">
-        <v>375</v>
+        <v>761</v>
       </c>
     </row>
     <row r="267" spans="1:11" ht="20" customHeight="1">
@@ -13333,33 +13424,392 @@
         <v>259</v>
       </c>
       <c r="B267" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="C267" s="9" t="s">
+        <v>566</v>
+      </c>
+      <c r="D267" s="9" t="s">
+        <v>574</v>
+      </c>
+      <c r="E267" s="16" t="s">
+        <v>558</v>
+      </c>
+      <c r="F267" s="21" t="s">
+        <v>755</v>
+      </c>
+      <c r="G267" s="21" t="s">
+        <v>756</v>
+      </c>
+      <c r="H267" s="9" t="s">
+        <v>762</v>
+      </c>
+      <c r="I267" s="8"/>
+      <c r="J267" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="K267" s="8" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="268" spans="1:11" ht="20" customHeight="1">
+      <c r="A268" s="6">
+        <v>260</v>
+      </c>
+      <c r="B268" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="C268" s="9" t="s">
+        <v>566</v>
+      </c>
+      <c r="D268" s="9" t="s">
+        <v>574</v>
+      </c>
+      <c r="E268" s="16" t="s">
+        <v>558</v>
+      </c>
+      <c r="F268" s="21" t="s">
+        <v>757</v>
+      </c>
+      <c r="G268" s="21" t="s">
+        <v>758</v>
+      </c>
+      <c r="H268" s="9" t="s">
+        <v>762</v>
+      </c>
+      <c r="I268" s="8"/>
+      <c r="J268" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="K268" s="8" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="269" spans="1:11" ht="20" customHeight="1">
+      <c r="A269" s="6">
+        <v>261</v>
+      </c>
+      <c r="B269" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="C269" s="9" t="s">
+        <v>566</v>
+      </c>
+      <c r="D269" s="9" t="s">
+        <v>574</v>
+      </c>
+      <c r="E269" s="16" t="s">
+        <v>558</v>
+      </c>
+      <c r="F269" s="21" t="s">
+        <v>759</v>
+      </c>
+      <c r="G269" s="21" t="s">
+        <v>760</v>
+      </c>
+      <c r="H269" s="9" t="s">
+        <v>762</v>
+      </c>
+      <c r="I269" s="8"/>
+      <c r="J269" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="K269" s="8" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="270" spans="1:11" ht="20" customHeight="1">
+      <c r="A270" s="6">
+        <v>262</v>
+      </c>
+      <c r="B270" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="C270" s="9" t="s">
+        <v>566</v>
+      </c>
+      <c r="D270" s="9" t="s">
+        <v>574</v>
+      </c>
+      <c r="E270" s="16" t="s">
+        <v>558</v>
+      </c>
+      <c r="F270" s="21" t="s">
+        <v>763</v>
+      </c>
+      <c r="G270" s="21" t="s">
+        <v>764</v>
+      </c>
+      <c r="H270" s="9" t="s">
+        <v>765</v>
+      </c>
+      <c r="I270" s="8"/>
+      <c r="J270" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="K270" s="8" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="271" spans="1:11" ht="20" customHeight="1">
+      <c r="A271" s="6">
+        <v>263</v>
+      </c>
+      <c r="B271" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="C271" s="9" t="s">
+        <v>566</v>
+      </c>
+      <c r="D271" s="9" t="s">
+        <v>574</v>
+      </c>
+      <c r="E271" s="16" t="s">
+        <v>558</v>
+      </c>
+      <c r="F271" s="21" t="s">
+        <v>766</v>
+      </c>
+      <c r="G271" s="21" t="s">
+        <v>767</v>
+      </c>
+      <c r="H271" s="9" t="s">
+        <v>669</v>
+      </c>
+      <c r="I271" s="8"/>
+      <c r="J271" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="K271" s="8" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="272" spans="1:11" ht="20" customHeight="1">
+      <c r="A272" s="6">
+        <v>264</v>
+      </c>
+      <c r="B272" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="C272" s="9" t="s">
+        <v>566</v>
+      </c>
+      <c r="D272" s="9" t="s">
+        <v>574</v>
+      </c>
+      <c r="E272" s="16" t="s">
+        <v>558</v>
+      </c>
+      <c r="F272" s="21" t="s">
+        <v>768</v>
+      </c>
+      <c r="G272" s="21" t="s">
+        <v>769</v>
+      </c>
+      <c r="H272" s="9"/>
+      <c r="I272" s="8"/>
+      <c r="J272" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="K272" s="8" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="273" spans="1:11" ht="20" customHeight="1">
+      <c r="A273" s="6">
+        <v>265</v>
+      </c>
+      <c r="B273" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="C273" s="9" t="s">
+        <v>566</v>
+      </c>
+      <c r="D273" s="9" t="s">
+        <v>574</v>
+      </c>
+      <c r="E273" s="16" t="s">
+        <v>558</v>
+      </c>
+      <c r="F273" s="21" t="s">
+        <v>770</v>
+      </c>
+      <c r="G273" s="21" t="s">
+        <v>771</v>
+      </c>
+      <c r="H273" s="9"/>
+      <c r="I273" s="8"/>
+      <c r="J273" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="K273" s="8" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="274" spans="1:11" ht="20" customHeight="1">
+      <c r="A274" s="6">
+        <v>266</v>
+      </c>
+      <c r="B274" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="C274" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="D274" s="17" t="s">
+        <v>558</v>
+      </c>
+      <c r="E274" s="17" t="s">
+        <v>558</v>
+      </c>
+      <c r="F274" s="21" t="s">
+        <v>381</v>
+      </c>
+      <c r="G274" s="21" t="s">
+        <v>378</v>
+      </c>
+      <c r="H274" s="9"/>
+      <c r="I274" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="J274" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="K274" s="8" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="275" spans="1:11" ht="20" customHeight="1">
+      <c r="A275" s="6">
+        <v>267</v>
+      </c>
+      <c r="B275" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="C275" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="D275" s="17" t="s">
+        <v>558</v>
+      </c>
+      <c r="E275" s="17" t="s">
+        <v>558</v>
+      </c>
+      <c r="F275" s="21" t="s">
+        <v>382</v>
+      </c>
+      <c r="G275" s="21" t="s">
+        <v>379</v>
+      </c>
+      <c r="H275" s="9"/>
+      <c r="I275" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="J275" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="K275" s="8" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="276" spans="1:11" ht="20" customHeight="1">
+      <c r="A276" s="6">
+        <v>268</v>
+      </c>
+      <c r="B276" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="C276" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="D276" s="17" t="s">
+        <v>558</v>
+      </c>
+      <c r="E276" s="17" t="s">
+        <v>558</v>
+      </c>
+      <c r="F276" s="21" t="s">
+        <v>377</v>
+      </c>
+      <c r="G276" s="21" t="s">
+        <v>380</v>
+      </c>
+      <c r="H276" s="9"/>
+      <c r="I276" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="J276" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="K276" s="8" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="277" spans="1:11" ht="20" customHeight="1">
+      <c r="A277" s="6">
+        <v>269</v>
+      </c>
+      <c r="B277" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="C277" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="D277" s="17" t="s">
+        <v>558</v>
+      </c>
+      <c r="E277" s="17" t="s">
+        <v>558</v>
+      </c>
+      <c r="F277" s="21" t="s">
+        <v>384</v>
+      </c>
+      <c r="G277" s="21" t="s">
+        <v>385</v>
+      </c>
+      <c r="H277" s="9"/>
+      <c r="I277" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="J277" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="K277" s="8" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="278" spans="1:11" ht="20" customHeight="1">
+      <c r="A278" s="6">
+        <v>270</v>
+      </c>
+      <c r="B278" s="7" t="s">
         <v>304</v>
       </c>
-      <c r="C267" s="9" t="s">
+      <c r="C278" s="9" t="s">
         <v>305</v>
       </c>
-      <c r="D267" s="17" t="s">
-        <v>558</v>
-      </c>
-      <c r="E267" s="17" t="s">
-        <v>558</v>
-      </c>
-      <c r="F267" s="19" t="s">
+      <c r="D278" s="17" t="s">
+        <v>558</v>
+      </c>
+      <c r="E278" s="17" t="s">
+        <v>558</v>
+      </c>
+      <c r="F278" s="19" t="s">
         <v>306</v>
       </c>
-      <c r="G267" s="19" t="s">
+      <c r="G278" s="19" t="s">
         <v>307</v>
       </c>
-      <c r="H267" s="9" t="s">
+      <c r="H278" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="I267" s="9" t="s">
+      <c r="I278" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="J267" s="9" t="s">
+      <c r="J278" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="K267" s="9" t="s">
+      <c r="K278" s="9" t="s">
         <v>309</v>
       </c>
     </row>

</xml_diff>